<commit_message>
Update REPARTITION DES LED SUR LE DISQUE GENEREE.xlsx
</commit_message>
<xml_diff>
--- a/REPARTITION DES LED SUR LE DISQUE GENEREE.xlsx
+++ b/REPARTITION DES LED SUR LE DISQUE GENEREE.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Afficheur rotatif\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tich\Pictures\POV_Display_MGPFV2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27810" windowHeight="13020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27810" windowHeight="13020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="194">
   <si>
     <t>P001</t>
   </si>
@@ -173,9 +174,6 @@
     <t>P048</t>
   </si>
   <si>
-    <t>P049</t>
-  </si>
-  <si>
     <t>P050</t>
   </si>
   <si>
@@ -191,9 +189,6 @@
     <t>P054</t>
   </si>
   <si>
-    <t>P055</t>
-  </si>
-  <si>
     <t>P056</t>
   </si>
   <si>
@@ -203,9 +198,6 @@
     <t>P062</t>
   </si>
   <si>
-    <t>P061</t>
-  </si>
-  <si>
     <t>P060</t>
   </si>
   <si>
@@ -224,9 +216,6 @@
     <t>P068</t>
   </si>
   <si>
-    <t>P067</t>
-  </si>
-  <si>
     <t>P066</t>
   </si>
   <si>
@@ -248,9 +237,6 @@
     <t>P073</t>
   </si>
   <si>
-    <t>P074</t>
-  </si>
-  <si>
     <t>P075</t>
   </si>
   <si>
@@ -275,9 +261,6 @@
     <t>P083</t>
   </si>
   <si>
-    <t>P082</t>
-  </si>
-  <si>
     <t>P081</t>
   </si>
   <si>
@@ -296,9 +279,6 @@
     <t>P089</t>
   </si>
   <si>
-    <t>P090</t>
-  </si>
-  <si>
     <t>P91</t>
   </si>
   <si>
@@ -320,9 +300,6 @@
     <t>P097</t>
   </si>
   <si>
-    <t>P098</t>
-  </si>
-  <si>
     <t>P099</t>
   </si>
   <si>
@@ -410,21 +387,9 @@
     <t>P128</t>
   </si>
   <si>
-    <t>P131</t>
-  </si>
-  <si>
-    <t>P130</t>
-  </si>
-  <si>
     <t>P129</t>
   </si>
   <si>
-    <t>P132</t>
-  </si>
-  <si>
-    <t>P133</t>
-  </si>
-  <si>
     <t>P134</t>
   </si>
   <si>
@@ -516,18 +481,6 @@
   </si>
   <si>
     <t>P162</t>
-  </si>
-  <si>
-    <t>P169</t>
-  </si>
-  <si>
-    <t>P168</t>
-  </si>
-  <si>
-    <t>P167</t>
-  </si>
-  <si>
-    <t>P166</t>
   </si>
   <si>
     <t>P165</t>
@@ -637,6 +590,28 @@
   </si>
   <si>
     <t>NB SECTEUR</t>
+  </si>
+  <si>
+    <t>P98</t>
+  </si>
+  <si>
+    <t>P074
+P049</t>
+  </si>
+  <si>
+    <t>P055
+P082</t>
+  </si>
+  <si>
+    <t>P061
+P090</t>
+  </si>
+  <si>
+    <t>P098
+P067</t>
+  </si>
+  <si>
+    <t>groupe de led</t>
   </si>
 </sst>
 </file>
@@ -688,7 +663,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -743,8 +718,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="darkDown">
+        <fgColor rgb="FFFF66FF"/>
+        <bgColor rgb="FFFF66FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="darkDown">
+        <fgColor rgb="FF00FFFF"/>
+        <bgColor rgb="FF00B0F0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="darkUp">
+        <fgColor rgb="FF00FFFF"/>
+        <bgColor rgb="FF00B0F0"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -770,11 +763,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalDown="1">
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal style="thin">
+        <color auto="1"/>
+      </diagonal>
+    </border>
+    <border diagonalUp="1">
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal style="thin">
+        <color auto="1"/>
+      </diagonal>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -881,6 +892,23 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -889,8 +917,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF00FFFF"/>
       <color rgb="FFFF66FF"/>
-      <color rgb="FF00FFFF"/>
+      <color rgb="FFFF00FF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1169,8 +1198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
-      <selection activeCell="X15" sqref="X15"/>
+    <sheetView topLeftCell="A7" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
+      <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1180,7 +1209,7 @@
   <sheetData>
     <row r="1" spans="1:29" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="24" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
@@ -1190,100 +1219,100 @@
     <row r="2" spans="1:29" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:29" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="20" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q3" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="R3" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="S3" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="T3" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="U3" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="V3" s="18" t="s">
         <v>172</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="W3" s="18" t="s">
         <v>173</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="X3" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="Y3" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="Z3" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="AA3" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="AB3" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="AC3" s="16" t="s">
         <v>179</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="Q3" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="R3" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="S3" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="T3" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="U3" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="V3" s="18" t="s">
-        <v>188</v>
-      </c>
-      <c r="W3" s="18" t="s">
-        <v>189</v>
-      </c>
-      <c r="X3" s="14" t="s">
-        <v>190</v>
-      </c>
-      <c r="Y3" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="Z3" s="14" t="s">
-        <v>192</v>
-      </c>
-      <c r="AA3" s="16" t="s">
-        <v>193</v>
-      </c>
-      <c r="AB3" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="AC3" s="16" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:29" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="22" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
       <c r="E5" s="23"/>
       <c r="S5" s="22" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1343,55 +1372,57 @@
       </c>
       <c r="B7" s="19"/>
       <c r="H7" s="16" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>203</v>
+        <v>187</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>100</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="35">
         <v>2</v>
       </c>
-      <c r="E8" s="16" t="s">
-        <v>166</v>
-      </c>
+      <c r="E8" s="36"/>
       <c r="F8" s="16" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="I8" s="15" t="s">
-        <v>102</v>
+        <v>188</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="K8" s="14" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="L8" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="M8" s="16" t="s">
-        <v>140</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="M8" s="36"/>
       <c r="T8" s="26"/>
       <c r="U8" s="21" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="V8" s="21">
         <v>1</v>
@@ -1399,6 +1430,14 @@
       <c r="W8" s="1">
         <f t="shared" ref="W8:W13" si="0">288/V8</f>
         <v>288</v>
+      </c>
+      <c r="Z8" s="1">
+        <f>$Z$7/V8</f>
+        <v>100</v>
+      </c>
+      <c r="AA8" s="1">
+        <f>$AA$7/V8</f>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:29" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1406,41 +1445,41 @@
         <v>3</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>167</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>133</v>
+        <v>151</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>150</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="J9" s="18" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="K9" s="18" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L9" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="M9" s="14" t="s">
-        <v>106</v>
+        <v>93</v>
+      </c>
+      <c r="M9" s="16" t="s">
+        <v>124</v>
       </c>
       <c r="N9" s="16" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="T9" s="27"/>
       <c r="U9" s="21" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="V9" s="21">
         <v>8</v>
@@ -1448,29 +1487,35 @@
       <c r="W9" s="1">
         <f t="shared" si="0"/>
         <v>36</v>
+      </c>
+      <c r="Z9" s="1">
+        <f t="shared" ref="Z9:Z15" si="1">$Z$7/V9</f>
+        <v>12.5</v>
+      </c>
+      <c r="AA9" s="1">
+        <f t="shared" ref="AA9:AA15" si="2">$AA$7/V9</f>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:29" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="35">
         <v>4</v>
       </c>
-      <c r="C10" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>98</v>
+      <c r="C10" s="36"/>
+      <c r="D10" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>117</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I10" s="11" t="s">
         <v>44</v>
@@ -1482,20 +1527,18 @@
         <v>48</v>
       </c>
       <c r="L10" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="M10" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="N10" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="O10" s="16" t="s">
-        <v>142</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="M10" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="N10" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="O10" s="36"/>
       <c r="T10" s="28"/>
       <c r="U10" s="21" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="V10" s="21">
         <v>12</v>
@@ -1503,6 +1546,14 @@
       <c r="W10" s="1">
         <f t="shared" si="0"/>
         <v>24</v>
+      </c>
+      <c r="Z10" s="1">
+        <f t="shared" si="1"/>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="AA10" s="1">
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:29" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1510,16 +1561,16 @@
         <v>5</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>66</v>
+        <v>90</v>
+      </c>
+      <c r="F11" s="39" t="s">
+        <v>192</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>46</v>
@@ -1536,21 +1587,21 @@
       <c r="K11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="L11" s="10" t="s">
-        <v>49</v>
+      <c r="L11" s="38" t="s">
+        <v>189</v>
       </c>
       <c r="M11" s="13" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="N11" s="14" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="O11" s="16" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="T11" s="29"/>
       <c r="U11" s="21" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="V11" s="21">
         <v>24</v>
@@ -1558,6 +1609,14 @@
       <c r="W11" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
+      </c>
+      <c r="Z11" s="1">
+        <f t="shared" si="1"/>
+        <v>4.166666666666667</v>
+      </c>
+      <c r="AA11" s="1">
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:29" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1565,13 +1624,13 @@
         <v>6</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>47</v>
@@ -1595,17 +1654,17 @@
         <v>29</v>
       </c>
       <c r="M12" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N12" s="13" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="O12" s="14" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="T12" s="30"/>
       <c r="U12" s="21" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="V12" s="21">
         <v>24</v>
@@ -1613,6 +1672,14 @@
       <c r="W12" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
+      </c>
+      <c r="Z12" s="1">
+        <f t="shared" si="1"/>
+        <v>4.166666666666667</v>
+      </c>
+      <c r="AA12" s="1">
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:29" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1620,16 +1687,16 @@
         <v>7</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>42</v>
@@ -1653,20 +1720,20 @@
         <v>30</v>
       </c>
       <c r="M13" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N13" s="13" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="O13" s="14" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="P13" s="16" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="T13" s="31"/>
       <c r="U13" s="21" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="V13" s="21">
         <v>32</v>
@@ -1677,6 +1744,14 @@
       </c>
       <c r="X13" s="1">
         <v>28</v>
+      </c>
+      <c r="Z13" s="1">
+        <f t="shared" si="1"/>
+        <v>3.125</v>
+      </c>
+      <c r="AA13" s="1">
+        <f t="shared" si="2"/>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:29" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1684,16 +1759,16 @@
         <v>8</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>37</v>
@@ -1717,30 +1792,35 @@
         <v>31</v>
       </c>
       <c r="M14" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N14" s="13" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="O14" s="14" t="s">
-        <v>10</v>
+        <v>98</v>
       </c>
       <c r="P14" s="16" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="T14" s="32"/>
       <c r="U14" s="21" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="V14" s="21">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="W14" s="1">
         <f>288/V14</f>
-        <v>8</v>
-      </c>
-      <c r="X14" s="1">
-        <v>32</v>
+        <v>9</v>
+      </c>
+      <c r="Z14" s="1">
+        <f t="shared" si="1"/>
+        <v>3.125</v>
+      </c>
+      <c r="AA14" s="1">
+        <f t="shared" si="2"/>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:29" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1748,16 +1828,16 @@
         <v>9</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>38</v>
@@ -1781,20 +1861,20 @@
         <v>32</v>
       </c>
       <c r="M15" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N15" s="13" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="O15" s="14" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="P15" s="16" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="T15" s="33"/>
       <c r="U15" s="21" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="V15" s="21">
         <v>32</v>
@@ -1802,6 +1882,14 @@
       <c r="W15" s="1">
         <f>288/V15</f>
         <v>9</v>
+      </c>
+      <c r="Z15" s="1">
+        <f t="shared" si="1"/>
+        <v>3.125</v>
+      </c>
+      <c r="AA15" s="1">
+        <f t="shared" si="2"/>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:29" ht="56.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -1809,13 +1897,13 @@
         <v>10</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>39</v>
@@ -1839,23 +1927,23 @@
         <v>33</v>
       </c>
       <c r="M16" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N16" s="13" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="O16" s="14" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="T16" s="21" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="U16" s="21" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="V16" s="34">
         <f>SUM(V8:V15)</f>
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1863,16 +1951,16 @@
         <v>11</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>59</v>
+        <v>84</v>
+      </c>
+      <c r="F17" s="38" t="s">
+        <v>191</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>40</v>
@@ -1889,145 +1977,137 @@
       <c r="K17" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="L17" s="10" t="s">
-        <v>55</v>
+      <c r="L17" s="39" t="s">
+        <v>190</v>
       </c>
       <c r="M17" s="13" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="N17" s="14" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="O17" s="16" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="35">
         <v>12</v>
       </c>
-      <c r="C18" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>90</v>
+      <c r="C18" s="36"/>
+      <c r="D18" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>109</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K18" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L18" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="M18" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="N18" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="O18" s="16" t="s">
-        <v>148</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="M18" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="N18" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="O18" s="36"/>
     </row>
     <row r="19" spans="1:15" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="35">
         <v>13</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>123</v>
+        <v>148</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>140</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K19" s="13" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="L19" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="M19" s="14" t="s">
-        <v>115</v>
+        <v>10</v>
+      </c>
+      <c r="M19" s="16" t="s">
+        <v>134</v>
       </c>
       <c r="N19" s="16" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="35">
         <v>14</v>
       </c>
-      <c r="E20" s="16" t="s">
-        <v>157</v>
-      </c>
+      <c r="E20" s="36"/>
       <c r="F20" s="16" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="I20" s="14" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="J20" s="14" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="K20" s="14" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="L20" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="M20" s="16" t="s">
-        <v>150</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="M20" s="36"/>
     </row>
     <row r="21" spans="1:15" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="35">
         <v>15</v>
       </c>
       <c r="H21" s="16" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="I21" s="16" t="s">
-        <v>160</v>
+        <v>137</v>
       </c>
       <c r="J21" s="16" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2123,4 +2203,973 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:CW9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" style="40" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" style="41"/>
+    <col min="27" max="27" width="11.42578125" style="41"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A1" s="40" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+      <c r="N1" s="41">
+        <v>13</v>
+      </c>
+      <c r="O1">
+        <v>14</v>
+      </c>
+      <c r="P1">
+        <v>15</v>
+      </c>
+      <c r="Q1">
+        <v>16</v>
+      </c>
+      <c r="R1">
+        <v>17</v>
+      </c>
+      <c r="S1">
+        <v>18</v>
+      </c>
+      <c r="T1">
+        <v>19</v>
+      </c>
+      <c r="U1">
+        <v>20</v>
+      </c>
+      <c r="V1">
+        <v>21</v>
+      </c>
+      <c r="W1">
+        <v>22</v>
+      </c>
+      <c r="X1">
+        <v>23</v>
+      </c>
+      <c r="Y1">
+        <v>24</v>
+      </c>
+      <c r="Z1">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="41">
+        <v>26</v>
+      </c>
+      <c r="AB1">
+        <v>27</v>
+      </c>
+      <c r="AC1">
+        <v>28</v>
+      </c>
+      <c r="AD1">
+        <v>29</v>
+      </c>
+      <c r="AE1">
+        <v>30</v>
+      </c>
+      <c r="AF1">
+        <v>31</v>
+      </c>
+      <c r="AG1">
+        <v>32</v>
+      </c>
+      <c r="AH1">
+        <v>33</v>
+      </c>
+      <c r="AI1">
+        <v>34</v>
+      </c>
+      <c r="AJ1">
+        <v>35</v>
+      </c>
+      <c r="AK1">
+        <v>36</v>
+      </c>
+      <c r="AL1">
+        <v>37</v>
+      </c>
+      <c r="AM1">
+        <v>38</v>
+      </c>
+      <c r="AN1">
+        <v>39</v>
+      </c>
+      <c r="AO1">
+        <v>40</v>
+      </c>
+      <c r="AP1">
+        <v>41</v>
+      </c>
+      <c r="AQ1">
+        <v>42</v>
+      </c>
+      <c r="AR1">
+        <v>43</v>
+      </c>
+      <c r="AS1">
+        <v>44</v>
+      </c>
+      <c r="AT1">
+        <v>45</v>
+      </c>
+      <c r="AU1">
+        <v>46</v>
+      </c>
+      <c r="AV1">
+        <v>47</v>
+      </c>
+      <c r="AW1">
+        <v>48</v>
+      </c>
+      <c r="AX1">
+        <v>49</v>
+      </c>
+      <c r="AY1">
+        <v>50</v>
+      </c>
+      <c r="AZ1">
+        <v>51</v>
+      </c>
+      <c r="BA1">
+        <v>52</v>
+      </c>
+      <c r="BB1">
+        <v>53</v>
+      </c>
+      <c r="BC1">
+        <v>54</v>
+      </c>
+      <c r="BD1">
+        <v>55</v>
+      </c>
+      <c r="BE1">
+        <v>56</v>
+      </c>
+      <c r="BF1">
+        <v>57</v>
+      </c>
+      <c r="BG1">
+        <v>58</v>
+      </c>
+      <c r="BH1">
+        <v>59</v>
+      </c>
+      <c r="BI1">
+        <v>60</v>
+      </c>
+      <c r="BJ1">
+        <v>61</v>
+      </c>
+      <c r="BK1">
+        <v>62</v>
+      </c>
+      <c r="BL1">
+        <v>63</v>
+      </c>
+      <c r="BM1">
+        <v>64</v>
+      </c>
+      <c r="BN1">
+        <v>65</v>
+      </c>
+      <c r="BO1">
+        <v>66</v>
+      </c>
+      <c r="BP1">
+        <v>67</v>
+      </c>
+      <c r="BQ1">
+        <v>68</v>
+      </c>
+      <c r="BR1">
+        <v>69</v>
+      </c>
+      <c r="BS1">
+        <v>70</v>
+      </c>
+      <c r="BT1">
+        <v>71</v>
+      </c>
+      <c r="BU1">
+        <v>72</v>
+      </c>
+      <c r="BV1">
+        <v>73</v>
+      </c>
+      <c r="BW1">
+        <v>74</v>
+      </c>
+      <c r="BX1">
+        <v>75</v>
+      </c>
+      <c r="BY1">
+        <v>76</v>
+      </c>
+      <c r="BZ1">
+        <v>77</v>
+      </c>
+      <c r="CA1">
+        <v>78</v>
+      </c>
+      <c r="CB1">
+        <v>79</v>
+      </c>
+      <c r="CC1">
+        <v>80</v>
+      </c>
+      <c r="CD1">
+        <v>81</v>
+      </c>
+      <c r="CE1">
+        <v>82</v>
+      </c>
+      <c r="CF1">
+        <v>83</v>
+      </c>
+      <c r="CG1">
+        <v>84</v>
+      </c>
+      <c r="CH1">
+        <v>85</v>
+      </c>
+      <c r="CI1">
+        <v>86</v>
+      </c>
+      <c r="CJ1">
+        <v>87</v>
+      </c>
+      <c r="CK1">
+        <v>88</v>
+      </c>
+      <c r="CL1">
+        <v>89</v>
+      </c>
+      <c r="CM1">
+        <v>90</v>
+      </c>
+      <c r="CN1">
+        <v>91</v>
+      </c>
+      <c r="CO1">
+        <v>92</v>
+      </c>
+      <c r="CP1">
+        <v>93</v>
+      </c>
+      <c r="CQ1">
+        <v>94</v>
+      </c>
+      <c r="CR1">
+        <v>95</v>
+      </c>
+      <c r="CS1">
+        <v>96</v>
+      </c>
+      <c r="CT1">
+        <v>97</v>
+      </c>
+      <c r="CU1">
+        <v>98</v>
+      </c>
+      <c r="CV1">
+        <v>99</v>
+      </c>
+      <c r="CW1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A2" s="40">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>0</v>
+      </c>
+      <c r="R2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S2" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" t="s">
+        <v>0</v>
+      </c>
+      <c r="U2" t="s">
+        <v>0</v>
+      </c>
+      <c r="V2" t="s">
+        <v>0</v>
+      </c>
+      <c r="W2" t="s">
+        <v>0</v>
+      </c>
+      <c r="X2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>0</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>0</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>0</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>0</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>0</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>0</v>
+      </c>
+      <c r="CF2" t="s">
+        <v>0</v>
+      </c>
+      <c r="CG2" t="s">
+        <v>0</v>
+      </c>
+      <c r="CH2" t="s">
+        <v>0</v>
+      </c>
+      <c r="CI2" t="s">
+        <v>0</v>
+      </c>
+      <c r="CJ2" t="s">
+        <v>0</v>
+      </c>
+      <c r="CK2" t="s">
+        <v>0</v>
+      </c>
+      <c r="CL2" t="s">
+        <v>0</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>0</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>0</v>
+      </c>
+      <c r="CO2" t="s">
+        <v>0</v>
+      </c>
+      <c r="CP2" t="s">
+        <v>0</v>
+      </c>
+      <c r="CQ2" t="s">
+        <v>0</v>
+      </c>
+      <c r="CR2" t="s">
+        <v>0</v>
+      </c>
+      <c r="CS2" t="s">
+        <v>0</v>
+      </c>
+      <c r="CT2" t="s">
+        <v>0</v>
+      </c>
+      <c r="CU2" t="s">
+        <v>0</v>
+      </c>
+      <c r="CV2" t="s">
+        <v>0</v>
+      </c>
+      <c r="CW2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A3" s="40">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" s="41" t="s">
+        <v>2</v>
+      </c>
+      <c r="O3" t="s">
+        <v>2</v>
+      </c>
+      <c r="P3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R3" t="s">
+        <v>2</v>
+      </c>
+      <c r="S3" t="s">
+        <v>2</v>
+      </c>
+      <c r="T3" t="s">
+        <v>2</v>
+      </c>
+      <c r="U3" t="s">
+        <v>2</v>
+      </c>
+      <c r="V3" t="s">
+        <v>2</v>
+      </c>
+      <c r="W3" t="s">
+        <v>2</v>
+      </c>
+      <c r="X3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AM3" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="AN3" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="AO3" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="AP3" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="AQ3" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="AR3" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="AS3" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="AT3" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="AU3" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="AV3" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="AW3" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="AX3" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="AY3" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="AZ3" t="s">
+        <v>5</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>5</v>
+      </c>
+      <c r="BB3" t="s">
+        <v>5</v>
+      </c>
+      <c r="BC3" t="s">
+        <v>5</v>
+      </c>
+      <c r="BD3" t="s">
+        <v>5</v>
+      </c>
+      <c r="BE3" t="s">
+        <v>5</v>
+      </c>
+      <c r="BF3" t="s">
+        <v>5</v>
+      </c>
+      <c r="BG3" t="s">
+        <v>5</v>
+      </c>
+      <c r="BH3" t="s">
+        <v>5</v>
+      </c>
+      <c r="BI3" t="s">
+        <v>5</v>
+      </c>
+      <c r="BJ3" t="s">
+        <v>5</v>
+      </c>
+      <c r="BK3" t="s">
+        <v>5</v>
+      </c>
+      <c r="BL3" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="BM3" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="BN3" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="BO3" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="BP3" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="BQ3" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="BR3" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="BS3" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="BT3" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="BU3" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="BV3" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="BW3" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="BX3" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="BY3" t="s">
+        <v>7</v>
+      </c>
+      <c r="BZ3" t="s">
+        <v>7</v>
+      </c>
+      <c r="CA3" t="s">
+        <v>7</v>
+      </c>
+      <c r="CB3" t="s">
+        <v>7</v>
+      </c>
+      <c r="CC3" t="s">
+        <v>7</v>
+      </c>
+      <c r="CD3" t="s">
+        <v>7</v>
+      </c>
+      <c r="CE3" t="s">
+        <v>7</v>
+      </c>
+      <c r="CF3" t="s">
+        <v>7</v>
+      </c>
+      <c r="CG3" t="s">
+        <v>7</v>
+      </c>
+      <c r="CH3" t="s">
+        <v>7</v>
+      </c>
+      <c r="CI3" t="s">
+        <v>7</v>
+      </c>
+      <c r="CJ3" t="s">
+        <v>7</v>
+      </c>
+      <c r="CK3" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="CL3" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="CM3" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="CN3" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="CO3" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="CP3" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="CQ3" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="CR3" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="CS3" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="CT3" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="CU3" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="CV3" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="CW3" s="42" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A4" s="40">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A5" s="40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A6" s="40">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A7" s="40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A8" s="40">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A9" s="40">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>